<commit_message>
First version of pipeline development with 6 use cases
</commit_message>
<xml_diff>
--- a/GridSearchCV_results/CKD_case/test_results_y_pred_clf_fpipe_a.xlsx
+++ b/GridSearchCV_results/CKD_case/test_results_y_pred_clf_fpipe_a.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epedufi-my.sharepoint.com/personal/pedro_morenosanchez_seamk_fi/Documents/SeAMK/GitHub/FeatureSelection_Classifier_Pipeline/GridSearchCV_results/CKD_case/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_D5CEDCC997D9AE9F8A1207D296494E1A4DC09FAE" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4493828B-26E8-4AB9-BF17-6139F98E6B85}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -49,8 +55,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,10 +108,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -113,6 +122,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -159,7 +176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -191,9 +208,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -225,6 +260,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -400,14 +453,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,30 +492,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="375" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C2">
-        <v>0.9833333333333333</v>
+        <v>0.98333333333333328</v>
       </c>
       <c r="D2">
-        <v>0.9782608695652174</v>
+        <v>0.97826086956521741</v>
       </c>
       <c r="E2">
-        <v>0.9574468085106383</v>
+        <v>0.95744680851063835</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>0.9733333333333334</v>
+        <v>0.97333333333333338</v>
       </c>
       <c r="H2">
-        <v>0.9866666666666667</v>
+        <v>0.98666666666666669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>